<commit_message>
ripup_channel changed, schedule::is(const timeslot t, const channel *c) added.
</commit_message>
<xml_diff>
--- a/Report/Bounds.xlsx
+++ b/Report/Bounds.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Bound</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>25x25</t>
+  </si>
+  <si>
+    <t>16x16</t>
   </si>
 </sst>
 </file>
@@ -222,6 +225,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -231,10 +238,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -541,11 +544,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:8">
@@ -878,19 +881,19 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="13">
         <f t="shared" si="1"/>
         <v>624</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="11">
         <f t="shared" si="5"/>
         <v>2709</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="12">
         <f t="shared" si="2"/>
         <v>3907</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="14">
         <f t="shared" si="3"/>
         <v>3907</v>
       </c>
@@ -904,23 +907,23 @@
         <v>900</v>
       </c>
       <c r="D14">
-        <f>SQRT(C14)</f>
+        <f t="shared" ref="D14:D26" si="6">SQRT(C14)</f>
         <v>30</v>
       </c>
-      <c r="E14" s="16">
-        <f>C14-1</f>
+      <c r="E14" s="13">
+        <f t="shared" ref="E14:E26" si="7">C14-1</f>
         <v>899</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="11">
         <f>ROUNDUP(D14^2*(D14+1)/6,0)</f>
         <v>4650</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="12">
         <f>ROUNDUP(D14^3/4,0)</f>
         <v>6750</v>
       </c>
-      <c r="H14" s="17">
-        <f>MAX(E14,F14,G14)</f>
+      <c r="H14" s="14">
+        <f t="shared" ref="H14:H26" si="8">MAX(E14,F14,G14)</f>
         <v>6750</v>
       </c>
     </row>
@@ -935,11 +938,11 @@
         <v>9</v>
       </c>
       <c r="D15">
-        <f>SQRT(C15)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E15" s="1">
-        <f>C15-1</f>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="F15" s="2">
@@ -951,7 +954,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="9">
-        <f>MAX(E15,F15,G15)</f>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
@@ -964,23 +967,23 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <f>SQRT(C16)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="E16" s="1">
-        <f>C16-1</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16:F26" si="6">ROUNDUP((D16^3-D16)/8,0)</f>
+        <f t="shared" ref="F16:F26" si="9">ROUNDUP((D16^3-D16)/8,0)</f>
         <v>8</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" ref="G16:G26" si="7">ROUNDUP((D16^3)/8,0)</f>
+        <f t="shared" ref="G16:G26" si="10">ROUNDUP((D16^3)/8,0)</f>
         <v>8</v>
       </c>
       <c r="H16" s="9">
-        <f>MAX(E16,F16,G16)</f>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
     </row>
@@ -993,23 +996,23 @@
         <v>25</v>
       </c>
       <c r="D17">
-        <f>SQRT(C17)</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="E17" s="1">
-        <f>C17-1</f>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="H17" s="9">
-        <f>MAX(E17,F17,G17)</f>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
     </row>
@@ -1022,23 +1025,23 @@
         <v>36</v>
       </c>
       <c r="D18">
-        <f>SQRT(C18)</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="E18" s="1">
-        <f>C18-1</f>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>27</v>
       </c>
       <c r="H18" s="9">
-        <f>MAX(E18,F18,G18)</f>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
     </row>
@@ -1051,23 +1054,23 @@
         <v>49</v>
       </c>
       <c r="D19">
-        <f>SQRT(C19)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="E19" s="1">
-        <f>C19-1</f>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>42</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>43</v>
       </c>
       <c r="H19" s="9">
-        <f>MAX(E19,F19,G19)</f>
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
     </row>
@@ -1080,23 +1083,23 @@
         <v>64</v>
       </c>
       <c r="D20">
-        <f>SQRT(C20)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="E20" s="1">
-        <f>C20-1</f>
+        <f t="shared" si="7"/>
         <v>63</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>63</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>64</v>
       </c>
       <c r="H20" s="9">
-        <f>MAX(E20,F20,G20)</f>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
     </row>
@@ -1109,23 +1112,23 @@
         <v>81</v>
       </c>
       <c r="D21">
-        <f>SQRT(C21)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="E21" s="1">
-        <f>C21-1</f>
+        <f t="shared" si="7"/>
         <v>80</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>92</v>
       </c>
       <c r="H21" s="9">
-        <f>MAX(E21,F21,G21)</f>
+        <f t="shared" si="8"/>
         <v>92</v>
       </c>
     </row>
@@ -1138,23 +1141,23 @@
         <v>100</v>
       </c>
       <c r="D22">
-        <f>SQRT(C22)</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="E22" s="1">
-        <f>C22-1</f>
+        <f t="shared" si="7"/>
         <v>99</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>124</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>125</v>
       </c>
       <c r="H22" s="9">
-        <f>MAX(E22,F22,G22)</f>
+        <f t="shared" si="8"/>
         <v>125</v>
       </c>
     </row>
@@ -1167,108 +1170,136 @@
         <v>225</v>
       </c>
       <c r="D23">
-        <f>SQRT(C23)</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="E23" s="1">
-        <f>C23-1</f>
+        <f t="shared" si="7"/>
         <v>224</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>420</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>422</v>
       </c>
       <c r="H23" s="9">
-        <f>MAX(E23,F23,G23)</f>
+        <f t="shared" si="8"/>
         <v>422</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>256</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="C24">
-        <v>400</v>
-      </c>
-      <c r="D24">
-        <f>SQRT(C24)</f>
-        <v>20</v>
-      </c>
-      <c r="E24" s="1">
-        <f>C24-1</f>
-        <v>399</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="6"/>
-        <v>998</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="E24" s="13">
         <f t="shared" si="7"/>
-        <v>1000</v>
-      </c>
-      <c r="H24" s="9">
-        <f>MAX(E24,F24,G24)</f>
-        <v>1000</v>
+        <v>255</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="9"/>
+        <v>510</v>
+      </c>
+      <c r="G24" s="12">
+        <f t="shared" si="10"/>
+        <v>512</v>
+      </c>
+      <c r="H24" s="14">
+        <f t="shared" si="8"/>
+        <v>512</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C25">
-        <v>625</v>
+        <v>400</v>
       </c>
       <c r="D25">
         <f>SQRT(C25)</f>
-        <v>25</v>
-      </c>
-      <c r="E25" s="16">
+        <v>20</v>
+      </c>
+      <c r="E25" s="1">
         <f>C25-1</f>
-        <v>624</v>
-      </c>
-      <c r="F25" s="14">
-        <f t="shared" si="6"/>
-        <v>1950</v>
-      </c>
-      <c r="G25" s="15">
-        <f t="shared" si="7"/>
-        <v>1954</v>
-      </c>
-      <c r="H25" s="17">
+        <v>399</v>
+      </c>
+      <c r="F25" s="2">
+        <f>ROUNDUP((D25^3-D25)/8,0)</f>
+        <v>998</v>
+      </c>
+      <c r="G25" s="3">
+        <f>ROUNDUP((D25^3)/8,0)</f>
+        <v>1000</v>
+      </c>
+      <c r="H25" s="9">
         <f>MAX(E25,F25,G25)</f>
-        <v>1954</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="B26" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26">
-        <v>900</v>
+        <v>625</v>
       </c>
       <c r="D26">
         <f>SQRT(C26)</f>
+        <v>25</v>
+      </c>
+      <c r="E26" s="13">
+        <f>C26-1</f>
+        <v>624</v>
+      </c>
+      <c r="F26" s="11">
+        <f>ROUNDUP((D26^3-D26)/8,0)</f>
+        <v>1950</v>
+      </c>
+      <c r="G26" s="12">
+        <f>ROUNDUP((D26^3)/8,0)</f>
+        <v>1954</v>
+      </c>
+      <c r="H26" s="14">
+        <f>MAX(E26,F26,G26)</f>
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27">
+        <v>900</v>
+      </c>
+      <c r="D27">
+        <f>SQRT(C27)</f>
         <v>30</v>
       </c>
-      <c r="E26" s="16">
-        <f>C26-1</f>
+      <c r="E27" s="13">
+        <f>C27-1</f>
         <v>899</v>
       </c>
-      <c r="F26" s="14">
-        <f t="shared" si="6"/>
+      <c r="F27" s="11">
+        <f>ROUNDUP((D27^3-D27)/8,0)</f>
         <v>3372</v>
       </c>
-      <c r="G26" s="15">
-        <f t="shared" si="7"/>
+      <c r="G27" s="12">
+        <f>ROUNDUP((D27^3)/8,0)</f>
         <v>3375</v>
       </c>
-      <c r="H26" s="17">
-        <f>MAX(E26,F26,G26)</f>
+      <c r="H27" s="14">
+        <f>MAX(E27,F27,G27)</f>
         <v>3375</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ALNS and GRASP are not safe to run
</commit_message>
<xml_diff>
--- a/Report/Bounds.xlsx
+++ b/Report/Bounds.xlsx
@@ -907,11 +907,11 @@
         <v>900</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D26" si="6">SQRT(C14)</f>
+        <f t="shared" ref="D14:D24" si="6">SQRT(C14)</f>
         <v>30</v>
       </c>
       <c r="E14" s="13">
-        <f t="shared" ref="E14:E26" si="7">C14-1</f>
+        <f t="shared" ref="E14:E24" si="7">C14-1</f>
         <v>899</v>
       </c>
       <c r="F14" s="11">
@@ -923,7 +923,7 @@
         <v>6750</v>
       </c>
       <c r="H14" s="14">
-        <f t="shared" ref="H14:H26" si="8">MAX(E14,F14,G14)</f>
+        <f t="shared" ref="H14:H24" si="8">MAX(E14,F14,G14)</f>
         <v>6750</v>
       </c>
     </row>
@@ -975,11 +975,11 @@
         <v>15</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16:F26" si="9">ROUNDUP((D16^3-D16)/8,0)</f>
+        <f t="shared" ref="F16:F24" si="9">ROUNDUP((D16^3-D16)/8,0)</f>
         <v>8</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" ref="G16:G26" si="10">ROUNDUP((D16^3)/8,0)</f>
+        <f t="shared" ref="G16:G24" si="10">ROUNDUP((D16^3)/8,0)</f>
         <v>8</v>
       </c>
       <c r="H16" s="9">

</xml_diff>